<commit_message>
forecast sheet update + FIM run
</commit_message>
<xml_diff>
--- a/results/04-2024/comparison-deflators-04-2024.xlsx
+++ b/results/04-2024/comparison-deflators-04-2024.xlsx
@@ -1339,22 +1339,22 @@
         <v>0.0699</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0612</v>
+        <v>-0.0599</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.056</v>
+        <v>-0.0547</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0552</v>
+        <v>-0.054</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.1095</v>
+        <v>-0.1083</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.0854</v>
+        <v>-0.0687</v>
       </c>
       <c r="W12" t="n">
-        <v>-6.3361</v>
+        <v>-6.3375</v>
       </c>
     </row>
     <row r="13">
@@ -1623,22 +1623,22 @@
         <v>-0.119</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.6875</v>
+        <v>-0.6862</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.8208</v>
+        <v>-0.8195</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.5654</v>
+        <v>-0.5642</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.3717</v>
+        <v>-0.3704</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.1076</v>
+        <v>-0.0909</v>
       </c>
       <c r="W16" t="n">
-        <v>-70.6457</v>
+        <v>-70.6471</v>
       </c>
     </row>
     <row r="17">
@@ -3327,22 +3327,22 @@
         <v>0.0997</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.0049</v>
+        <v>-0.0036</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.0047</v>
+        <v>-0.0034</v>
       </c>
       <c r="T40" t="n">
-        <v>-0.0046</v>
+        <v>-0.0034</v>
       </c>
       <c r="U40" t="n">
-        <v>-0.0045</v>
+        <v>-0.0033</v>
       </c>
       <c r="V40" t="n">
-        <v>6.2193</v>
+        <v>6.236</v>
       </c>
       <c r="W40" t="n">
-        <v>-0.139</v>
+        <v>-0.1405</v>
       </c>
     </row>
     <row r="41">
@@ -3611,22 +3611,22 @@
         <v>0.143</v>
       </c>
       <c r="R44" t="n">
-        <v>0.1216</v>
+        <v>0.1229</v>
       </c>
       <c r="S44" t="n">
-        <v>0.0048</v>
+        <v>0.0061</v>
       </c>
       <c r="T44" t="n">
-        <v>-0.0325</v>
+        <v>-0.0312</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.0281</v>
+        <v>-0.0269</v>
       </c>
       <c r="V44" t="n">
-        <v>50.6568</v>
+        <v>50.6734</v>
       </c>
       <c r="W44" t="n">
-        <v>-44.3669</v>
+        <v>-44.3683</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
feat: calculate 2024-04 FIM without MPCs and save in results/04-2024-no mpcs
</commit_message>
<xml_diff>
--- a/results/04-2024/comparison-deflators-04-2024.xlsx
+++ b/results/04-2024/comparison-deflators-04-2024.xlsx
@@ -614,10 +614,10 @@
         <v>0.0064</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0045</v>
+        <v>0.0044</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0065</v>
+        <v>0.0084</v>
       </c>
       <c r="O2" t="n">
         <v>0.0067</v>
@@ -688,7 +688,7 @@
         <v>308.099</v>
       </c>
       <c r="N3" t="n">
-        <v>313.446</v>
+        <v>310.9897</v>
       </c>
       <c r="O3" t="n">
         <v>315.355</v>
@@ -762,31 +762,31 @@
         <v>-0.0074</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.0185</v>
+        <v>-0.0177</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0698</v>
+        <v>-0.0669</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.0303</v>
+        <v>-0.029</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0293</v>
+        <v>-0.028</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.0276</v>
+        <v>-0.0264</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.0268</v>
+        <v>-0.0257</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.004</v>
+        <v>-0.0038</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.0028</v>
+        <v>-0.0026</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.0023</v>
+        <v>-0.0022</v>
       </c>
     </row>
     <row r="5">
@@ -827,37 +827,37 @@
         <v>-0.0421</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1515</v>
+        <v>0.1538</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.1397</v>
+        <v>-0.2668</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.3756</v>
+        <v>-0.3599</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.0703</v>
+        <v>-0.0673</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0875</v>
+        <v>-0.0838</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.4406</v>
+        <v>-0.4221</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.3113</v>
+        <v>-0.2982</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.1371</v>
+        <v>-0.1313</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.1743</v>
+        <v>-0.167</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.1107</v>
+        <v>-0.106</v>
       </c>
       <c r="W5" t="n">
-        <v>-32.7795</v>
+        <v>-31.4048</v>
       </c>
     </row>
     <row r="6">
@@ -898,37 +898,37 @@
         <v>0.3088</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4869</v>
+        <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1582</v>
+        <v>0.1561</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1284</v>
+        <v>-0.1203</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.2514</v>
+        <v>-0.2381</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.2362</v>
+        <v>-0.2235</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2991</v>
+        <v>-0.2839</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2319</v>
+        <v>-0.2195</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.1809</v>
+        <v>-0.1707</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.0397</v>
+        <v>-0.0354</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1218</v>
+        <v>-0.1141</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.4486</v>
+        <v>-0.4273</v>
       </c>
     </row>
     <row r="7">
@@ -969,37 +969,37 @@
         <v>-0.2751</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.1625</v>
+        <v>-0.1622</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.2067</v>
+        <v>-0.2224</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.175</v>
+        <v>-0.1833</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0571</v>
+        <v>0.0393</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0151</v>
+        <v>-0.0011</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0575</v>
+        <v>0.0551</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0467</v>
+        <v>0.0448</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0335</v>
+        <v>0.0321</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0505</v>
+        <v>0.0484</v>
       </c>
       <c r="V7" t="n">
-        <v>0.096</v>
+        <v>0.092</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.2441</v>
+        <v>-5.0242</v>
       </c>
     </row>
     <row r="8">
@@ -1040,37 +1040,37 @@
         <v>0.3669</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3655</v>
+        <v>0.3659</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1789</v>
+        <v>0.2014</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0917</v>
+        <v>0.11</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2734</v>
+        <v>0.273</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2064</v>
+        <v>0.2087</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1509</v>
+        <v>-0.1338</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.1694</v>
+        <v>-0.1517</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.1405</v>
+        <v>-0.1241</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.1332</v>
+        <v>-0.1174</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.0704</v>
+        <v>-0.0675</v>
       </c>
       <c r="W8" t="n">
-        <v>7.7895</v>
+        <v>7.4628</v>
       </c>
     </row>
     <row r="9">
@@ -1117,31 +1117,31 @@
         <v>-0.0373</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0373</v>
+        <v>-0.0357</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0359</v>
+        <v>-0.0344</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.0234</v>
+        <v>-0.0224</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0159</v>
+        <v>-0.0152</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.0144</v>
+        <v>-0.0138</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.0145</v>
+        <v>-0.0139</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.0135</v>
+        <v>-0.0129</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.0149</v>
+        <v>-0.0143</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.0102</v>
+        <v>-0.0097</v>
       </c>
     </row>
     <row r="10">
@@ -1185,34 +1185,34 @@
         <v>-0.0966</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.0619</v>
+        <v>-0.062</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.051</v>
+        <v>-0.0488</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.0451</v>
+        <v>-0.0433</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0269</v>
+        <v>-0.0258</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0107</v>
+        <v>-0.0103</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0102</v>
+        <v>-0.0098</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.0086</v>
+        <v>-0.0083</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.0078</v>
+        <v>-0.0075</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.0072</v>
+        <v>-0.0069</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.0066</v>
+        <v>-0.0063</v>
       </c>
     </row>
     <row r="11">
@@ -1253,10 +1253,10 @@
         <v>0.0098</v>
       </c>
       <c r="M11" t="n">
-        <v>0.01</v>
+        <v>0.0098</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0073</v>
+        <v>0.0101</v>
       </c>
       <c r="O11" t="n">
         <v>0.0078</v>
@@ -1324,37 +1324,37 @@
         <v>0.0114</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.1485</v>
+        <v>-0.1481</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0462</v>
+        <v>-0.0659</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0456</v>
+        <v>0.0242</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0891</v>
+        <v>0.0661</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0932</v>
+        <v>0.0699</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0625</v>
+        <v>-0.0599</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.0571</v>
+        <v>-0.0547</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0564</v>
+        <v>-0.054</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.113</v>
+        <v>-0.1083</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.0717</v>
+        <v>-0.0687</v>
       </c>
       <c r="W12" t="n">
-        <v>-6.615</v>
+        <v>-6.3375</v>
       </c>
     </row>
     <row r="13">
@@ -1398,22 +1398,22 @@
         <v>-0.1126</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.1019</v>
+        <v>-0.1018</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.0973</v>
+        <v>-0.0932</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.0573</v>
+        <v>-0.0549</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.0311</v>
+        <v>-0.0298</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.0308</v>
+        <v>-0.0295</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.0242</v>
+        <v>-0.0232</v>
       </c>
       <c r="T13" t="n">
         <v>0.0002</v>
@@ -1425,7 +1425,7 @@
         <v>-0.0001</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.0074</v>
+        <v>-0.0071</v>
       </c>
     </row>
     <row r="14">
@@ -1466,37 +1466,37 @@
         <v>-0.3432</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.1407</v>
+        <v>-0.1408</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.1051</v>
+        <v>-0.1042</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.3045</v>
+        <v>-0.292</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2741</v>
+        <v>-0.2628</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1105</v>
+        <v>-0.106</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0604</v>
+        <v>-0.0581</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0966</v>
+        <v>-0.0926</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0716</v>
+        <v>-0.0687</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.032</v>
+        <v>-0.0308</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0119</v>
+        <v>-0.0116</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.0755</v>
+        <v>-0.0725</v>
       </c>
     </row>
     <row r="15">
@@ -1540,31 +1540,31 @@
         <v>-0.0074</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.0027</v>
+        <v>-0.0014</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.0005</v>
+        <v>-0.0007</v>
       </c>
       <c r="P15" t="n">
         <v>-0.0003</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="R15" t="n">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="W15" t="n">
         <v>0</v>
@@ -1608,37 +1608,37 @@
         <v>0.5287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4702</v>
+        <v>0.2312</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1079</v>
+        <v>-0.2545</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.7326</v>
+        <v>-0.6738</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.3602</v>
+        <v>-0.363</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.0647</v>
+        <v>-0.119</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.797</v>
+        <v>-0.6862</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.8765</v>
+        <v>-0.8195</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.6097</v>
+        <v>-0.5642</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.4352</v>
+        <v>-0.3704</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.0983</v>
+        <v>-0.0909</v>
       </c>
       <c r="W16" t="n">
-        <v>-73.7432</v>
+        <v>-70.6471</v>
       </c>
     </row>
     <row r="17">
@@ -1679,37 +1679,37 @@
         <v>27610.1</v>
       </c>
       <c r="M17" t="n">
-        <v>27944.6</v>
+        <v>27957</v>
       </c>
       <c r="N17" t="n">
-        <v>27098.3</v>
+        <v>28284.5</v>
       </c>
       <c r="O17" t="n">
-        <v>27422.1</v>
+        <v>28622.474</v>
       </c>
       <c r="P17" t="n">
-        <v>27752.5</v>
+        <v>28967.3369</v>
       </c>
       <c r="Q17" t="n">
-        <v>28094.6</v>
+        <v>29324.412</v>
       </c>
       <c r="R17" t="n">
-        <v>28443.2</v>
+        <v>29688.2716</v>
       </c>
       <c r="S17" t="n">
-        <v>28783.5</v>
+        <v>30043.4679</v>
       </c>
       <c r="T17" t="n">
-        <v>29119</v>
+        <v>30393.654</v>
       </c>
       <c r="U17" t="n">
-        <v>29442.5</v>
+        <v>30731.3149</v>
       </c>
       <c r="V17" t="n">
-        <v>29766.2</v>
+        <v>31069.1846</v>
       </c>
       <c r="W17" t="n">
-        <v>30094.6</v>
+        <v>31411.9599</v>
       </c>
     </row>
     <row r="18">
@@ -1750,37 +1750,37 @@
         <v>-0.3502</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1484</v>
+        <v>0.1455</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.0895</v>
+        <v>-0.1094</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.2198</v>
+        <v>-0.2106</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0112</v>
+        <v>-0.0107</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0159</v>
+        <v>0.0152</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.3182</v>
+        <v>-0.3049</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.198</v>
+        <v>-0.1896</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.0381</v>
+        <v>-0.0365</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.0914</v>
+        <v>-0.0876</v>
       </c>
       <c r="V18" t="n">
-        <v>0.0075</v>
+        <v>0.0072</v>
       </c>
       <c r="W18" t="n">
-        <v>-6.5915</v>
+        <v>-6.3151</v>
       </c>
     </row>
     <row r="19">
@@ -1824,7 +1824,7 @@
         <v>0.0056</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0041</v>
+        <v>0.0055</v>
       </c>
       <c r="O19" t="n">
         <v>0.0041</v>
@@ -1898,28 +1898,28 @@
         <v>-0.1124</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.1096</v>
+        <v>-0.105</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.1064</v>
+        <v>-0.1019</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.1042</v>
+        <v>-0.0998</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.1009</v>
+        <v>-0.0967</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.0978</v>
+        <v>-0.0937</v>
       </c>
       <c r="T20" t="n">
-        <v>-0.0011</v>
+        <v>-0.001</v>
       </c>
       <c r="U20" t="n">
         <v>-0.001</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.001</v>
+        <v>-0.0009</v>
       </c>
       <c r="W20" t="n">
         <v>0</v>
@@ -2034,37 +2034,37 @@
         <v>0.6465</v>
       </c>
       <c r="M22" t="n">
-        <v>0.1846</v>
+        <v>0.2484</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2648</v>
+        <v>0.0936</v>
       </c>
       <c r="O22" t="n">
-        <v>0.1625</v>
+        <v>0.1557</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.0456</v>
+        <v>-0.0437</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.0653</v>
+        <v>-0.0625</v>
       </c>
       <c r="R22" t="n">
-        <v>0.2428</v>
+        <v>0.2326</v>
       </c>
       <c r="S22" t="n">
-        <v>0.1264</v>
+        <v>0.1211</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.0305</v>
+        <v>-0.0292</v>
       </c>
       <c r="U22" t="n">
-        <v>0.0168</v>
+        <v>0.0161</v>
       </c>
       <c r="V22" t="n">
-        <v>0.2029</v>
+        <v>0.1944</v>
       </c>
       <c r="W22" t="n">
-        <v>-38.744</v>
+        <v>-37.1192</v>
       </c>
     </row>
     <row r="23">
@@ -2105,37 +2105,37 @@
         <v>-0.0209</v>
       </c>
       <c r="M23" t="n">
-        <v>0.053</v>
+        <v>-0.027</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.0211</v>
+        <v>-0.02</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.0179</v>
+        <v>-0.016</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.0099</v>
+        <v>-0.0085</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.0076</v>
+        <v>0.0083</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0224</v>
+        <v>0.0225</v>
       </c>
       <c r="S23" t="n">
-        <v>0.0012</v>
+        <v>0.0022</v>
       </c>
       <c r="T23" t="n">
-        <v>0.0013</v>
+        <v>0.0023</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0067</v>
+        <v>0.0074</v>
       </c>
       <c r="V23" t="n">
-        <v>0.0113</v>
+        <v>0.0118</v>
       </c>
       <c r="W23" t="n">
-        <v>0.075</v>
+        <v>0.0729</v>
       </c>
     </row>
     <row r="24">
@@ -2176,37 +2176,37 @@
         <v>0.219</v>
       </c>
       <c r="M24" t="n">
-        <v>0.017</v>
+        <v>0.0574</v>
       </c>
       <c r="N24" t="n">
-        <v>0.1117</v>
+        <v>0.1087</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0319</v>
+        <v>0.0277</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.0257</v>
+        <v>-0.0275</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.1447</v>
+        <v>0.0972</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0062</v>
+        <v>-0.006</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.0206</v>
+        <v>-0.0198</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.0159</v>
+        <v>-0.0153</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.008</v>
+        <v>-0.0077</v>
       </c>
       <c r="V24" t="n">
-        <v>0.0049</v>
+        <v>0.0047</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.9329</v>
+        <v>-0.8938</v>
       </c>
     </row>
     <row r="25">
@@ -2247,37 +2247,37 @@
         <v>0.1954</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1982</v>
+        <v>0.1388</v>
       </c>
       <c r="N25" t="n">
-        <v>0.2255</v>
+        <v>0.2383</v>
       </c>
       <c r="O25" t="n">
-        <v>0.1977</v>
+        <v>0.2312</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1471</v>
+        <v>0.1473</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.1092</v>
+        <v>0.1108</v>
       </c>
       <c r="R25" t="n">
-        <v>0.0655</v>
+        <v>0.0689</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.012</v>
+        <v>-0.0054</v>
       </c>
       <c r="T25" t="n">
-        <v>0.017</v>
+        <v>0.0223</v>
       </c>
       <c r="U25" t="n">
-        <v>-0.0023</v>
+        <v>0.0307</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.023</v>
+        <v>-0.022</v>
       </c>
       <c r="W25" t="n">
-        <v>3.9993</v>
+        <v>3.8316</v>
       </c>
     </row>
     <row r="26">
@@ -2318,10 +2318,10 @@
         <v>0.0141</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0012</v>
+        <v>0.0016</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0077</v>
+        <v>0.009</v>
       </c>
       <c r="O26" t="n">
         <v>0.0071</v>
@@ -2392,7 +2392,7 @@
         <v>176.9</v>
       </c>
       <c r="N27" t="n">
-        <v>196.2983</v>
+        <v>177.9</v>
       </c>
       <c r="O27" t="n">
         <v>199.5248</v>
@@ -2463,25 +2463,25 @@
         <v>-0.0001</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.0011</v>
+        <v>-0.0006</v>
       </c>
       <c r="O28" t="n">
-        <v>-0.0027</v>
+        <v>-0.0026</v>
       </c>
       <c r="P28" t="n">
         <v>-0.0005</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0005</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.0006</v>
+        <v>-0.0007</v>
       </c>
       <c r="S28" t="n">
-        <v>-0.0014</v>
+        <v>-0.0013</v>
       </c>
       <c r="T28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0003</v>
       </c>
       <c r="U28" t="n">
         <v>-0.0003</v>
@@ -2534,34 +2534,34 @@
         <v>-0.0005</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.0012</v>
+        <v>-0.0027</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0046</v>
+        <v>0.0044</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0064</v>
+        <v>0.0061</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.006</v>
+        <v>0.0057</v>
       </c>
       <c r="R29" t="n">
         <v>0.0062</v>
       </c>
       <c r="S29" t="n">
-        <v>0.0064</v>
+        <v>0.0063</v>
       </c>
       <c r="T29" t="n">
-        <v>0.0052</v>
+        <v>0.0049</v>
       </c>
       <c r="U29" t="n">
-        <v>0.0025</v>
+        <v>0.0024</v>
       </c>
       <c r="V29" t="n">
-        <v>0.0011</v>
+        <v>0.0013</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.0743</v>
+        <v>-0.0712</v>
       </c>
     </row>
     <row r="30">
@@ -2602,10 +2602,10 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>-0.0009</v>
+        <v>0.001</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>
@@ -2676,7 +2676,7 @@
         <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>-2.4563</v>
       </c>
       <c r="O31" t="n">
         <v>0</v>
@@ -2750,31 +2750,31 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>-0.0008</v>
+        <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.0029</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.0013</v>
+        <v>0</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.0012</v>
+        <v>0</v>
       </c>
       <c r="S32" t="n">
-        <v>-0.0011</v>
+        <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>-0.0011</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="V32" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="W32" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2815,37 +2815,37 @@
         <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.0023</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>0.1163</v>
+        <v>-0.0109</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0867</v>
+        <v>0.1024</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.0033</v>
+        <v>-0.0004</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.0042</v>
+        <v>-0.0006</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.0191</v>
+        <v>-0.0006</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.0137</v>
+        <v>-0.0006</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.0064</v>
+        <v>-0.0006</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.0079</v>
+        <v>-0.0005</v>
       </c>
       <c r="V33" t="n">
-        <v>1.8324</v>
+        <v>1.8371</v>
       </c>
       <c r="W33" t="n">
-        <v>-3.3281</v>
+        <v>-1.9534</v>
       </c>
     </row>
     <row r="34">
@@ -2886,37 +2886,37 @@
         <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.2073</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.0009</v>
+        <v>-0.0031</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0077</v>
+        <v>0.0005</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.0128</v>
+        <v>0.0005</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.0121</v>
+        <v>0.0005</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.0147</v>
+        <v>0.0005</v>
       </c>
       <c r="S34" t="n">
-        <v>-0.0119</v>
+        <v>0.0005</v>
       </c>
       <c r="T34" t="n">
-        <v>-0.0097</v>
+        <v>0.0005</v>
       </c>
       <c r="U34" t="n">
-        <v>-0.0038</v>
+        <v>0.0004</v>
       </c>
       <c r="V34" t="n">
-        <v>0.6203</v>
+        <v>0.628</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.6461</v>
+        <v>-0.6247</v>
       </c>
     </row>
     <row r="35">
@@ -2957,37 +2957,37 @@
         <v>0</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0259</v>
+        <v>0.0102</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0443</v>
+        <v>0.036</v>
       </c>
       <c r="P35" t="n">
-        <v>0.077</v>
+        <v>0.0592</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.072</v>
+        <v>0.0558</v>
       </c>
       <c r="R35" t="n">
-        <v>0.0452</v>
+        <v>0.0428</v>
       </c>
       <c r="S35" t="n">
-        <v>0.0169</v>
+        <v>0.0149</v>
       </c>
       <c r="T35" t="n">
-        <v>-0.009</v>
+        <v>-0.0104</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.0054</v>
+        <v>-0.0075</v>
       </c>
       <c r="V35" t="n">
-        <v>0.0258</v>
+        <v>0.0218</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.2547</v>
+        <v>-0.0348</v>
       </c>
     </row>
     <row r="36">
@@ -3028,37 +3028,37 @@
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>-0.0663</v>
+        <v>-0.0438</v>
       </c>
       <c r="O36" t="n">
-        <v>-0.1156</v>
+        <v>-0.0973</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.0739</v>
+        <v>-0.0743</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.0489</v>
+        <v>-0.0467</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.0642</v>
+        <v>-0.0472</v>
       </c>
       <c r="S36" t="n">
-        <v>-0.0641</v>
+        <v>-0.0464</v>
       </c>
       <c r="T36" t="n">
-        <v>-0.0614</v>
+        <v>-0.045</v>
       </c>
       <c r="U36" t="n">
-        <v>-0.0601</v>
+        <v>-0.0443</v>
       </c>
       <c r="V36" t="n">
-        <v>-0.067</v>
+        <v>-0.064</v>
       </c>
       <c r="W36" t="n">
-        <v>0.3982</v>
+        <v>0.0715</v>
       </c>
     </row>
     <row r="37">
@@ -3105,31 +3105,31 @@
         <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>-0.0016</v>
+        <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.0015</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.001</v>
+        <v>0</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.0007</v>
+        <v>0</v>
       </c>
       <c r="S37" t="n">
-        <v>-0.0006</v>
+        <v>0</v>
       </c>
       <c r="T37" t="n">
-        <v>-0.0006</v>
+        <v>0</v>
       </c>
       <c r="U37" t="n">
-        <v>-0.0006</v>
+        <v>0</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.0006</v>
+        <v>0</v>
       </c>
       <c r="W37" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3176,31 +3176,31 @@
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>-0.0021</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>-0.0019</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="n">
-        <v>-0.0011</v>
+        <v>0</v>
       </c>
       <c r="R38" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="S38" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="T38" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="U38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="V38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="W38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3241,10 +3241,10 @@
         <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>0.0014</v>
+        <v>0.0042</v>
       </c>
       <c r="O39" t="n">
         <v>0.0015</v>
@@ -3312,37 +3312,37 @@
         <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0.1267</v>
+        <v>0.1071</v>
       </c>
       <c r="O40" t="n">
-        <v>0.1259</v>
+        <v>0.1045</v>
       </c>
       <c r="P40" t="n">
-        <v>0.1251</v>
+        <v>0.1021</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.123</v>
+        <v>0.0997</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.0062</v>
+        <v>-0.0036</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.0058</v>
+        <v>-0.0034</v>
       </c>
       <c r="T40" t="n">
-        <v>-0.0057</v>
+        <v>-0.0034</v>
       </c>
       <c r="U40" t="n">
-        <v>-0.0081</v>
+        <v>-0.0033</v>
       </c>
       <c r="V40" t="n">
-        <v>6.233</v>
+        <v>6.236</v>
       </c>
       <c r="W40" t="n">
-        <v>-0.4179</v>
+        <v>-0.1405</v>
       </c>
     </row>
     <row r="41">
@@ -3389,19 +3389,19 @@
         <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>-0.004</v>
+        <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>-0.0024</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="n">
-        <v>-0.0013</v>
+        <v>0</v>
       </c>
       <c r="R41" t="n">
-        <v>-0.0013</v>
+        <v>0</v>
       </c>
       <c r="S41" t="n">
-        <v>-0.001</v>
+        <v>0</v>
       </c>
       <c r="T41" t="n">
         <v>0</v>
@@ -3413,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="W41" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3454,37 +3454,37 @@
         <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="N42" t="n">
+        <v>-0.0007</v>
+      </c>
+      <c r="O42" t="n">
         <v>-0.0015</v>
       </c>
-      <c r="O42" t="n">
-        <v>-0.0139</v>
-      </c>
       <c r="P42" t="n">
-        <v>-0.0126</v>
+        <v>-0.0013</v>
       </c>
       <c r="Q42" t="n">
-        <v>-0.0057</v>
+        <v>-0.0012</v>
       </c>
       <c r="R42" t="n">
-        <v>-0.0034</v>
+        <v>-0.0011</v>
       </c>
       <c r="S42" t="n">
-        <v>-0.0049</v>
+        <v>-0.001</v>
       </c>
       <c r="T42" t="n">
-        <v>-0.0038</v>
+        <v>-0.001</v>
       </c>
       <c r="U42" t="n">
-        <v>-0.0022</v>
+        <v>-0.001</v>
       </c>
       <c r="V42" t="n">
-        <v>0.0659</v>
+        <v>0.0662</v>
       </c>
       <c r="W42" t="n">
-        <v>-0.0118</v>
+        <v>-0.0087</v>
       </c>
     </row>
     <row r="43">
@@ -3528,31 +3528,31 @@
         <v>0</v>
       </c>
       <c r="N43" t="n">
-        <v>-0.0013</v>
+        <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="P43" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q43" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="R43" t="n">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
       <c r="S43" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="T43" t="n">
         <v>0</v>
       </c>
       <c r="U43" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="V43" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="W43" t="n">
         <v>0</v>
@@ -3596,37 +3596,37 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.239</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0.3807</v>
+        <v>0.0184</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.0606</v>
+        <v>-0.0019</v>
       </c>
       <c r="P44" t="n">
-        <v>0.1255</v>
+        <v>0.1226</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.1973</v>
+        <v>0.143</v>
       </c>
       <c r="R44" t="n">
-        <v>0.0121</v>
+        <v>0.1229</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.0508</v>
+        <v>0.0061</v>
       </c>
       <c r="T44" t="n">
-        <v>-0.0768</v>
+        <v>-0.0312</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.0917</v>
+        <v>-0.0269</v>
       </c>
       <c r="V44" t="n">
-        <v>50.6661</v>
+        <v>50.6734</v>
       </c>
       <c r="W44" t="n">
-        <v>-47.4644</v>
+        <v>-44.3683</v>
       </c>
     </row>
     <row r="45">
@@ -3667,37 +3667,37 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>-12.4</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>-1178.4244</v>
+        <v>7.7756</v>
       </c>
       <c r="O45" t="n">
-        <v>-1192.5055</v>
+        <v>7.8685</v>
       </c>
       <c r="P45" t="n">
-        <v>-1206.8736</v>
+        <v>7.9633</v>
       </c>
       <c r="Q45" t="n">
-        <v>-1221.7505</v>
+        <v>8.0615</v>
       </c>
       <c r="R45" t="n">
-        <v>-1236.9101</v>
+        <v>8.1615</v>
       </c>
       <c r="S45" t="n">
-        <v>-1251.7088</v>
+        <v>8.2591</v>
       </c>
       <c r="T45" t="n">
-        <v>-1266.2987</v>
+        <v>8.3554</v>
       </c>
       <c r="U45" t="n">
-        <v>-1280.3667</v>
+        <v>8.4482</v>
       </c>
       <c r="V45" t="n">
-        <v>-1294.4435</v>
+        <v>8.5411</v>
       </c>
       <c r="W45" t="n">
-        <v>-1308.7246</v>
+        <v>8.6353</v>
       </c>
     </row>
     <row r="46">
@@ -3738,37 +3738,37 @@
         <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>0.0029</v>
+        <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>0.0295</v>
+        <v>0.0097</v>
       </c>
       <c r="O46" t="n">
-        <v>0.1319</v>
+        <v>0.1411</v>
       </c>
       <c r="P46" t="n">
-        <v>-0.0006</v>
+        <v>-0.0001</v>
       </c>
       <c r="Q46" t="n">
-        <v>0.0005</v>
+        <v>-0.0001</v>
       </c>
       <c r="R46" t="n">
-        <v>-0.0135</v>
+        <v>-0.0001</v>
       </c>
       <c r="S46" t="n">
-        <v>-0.0084</v>
+        <v>-0.0001</v>
       </c>
       <c r="T46" t="n">
-        <v>-0.0018</v>
+        <v>-0.0002</v>
       </c>
       <c r="U46" t="n">
-        <v>-0.004</v>
+        <v>-0.0002</v>
       </c>
       <c r="V46" t="n">
-        <v>1.7041</v>
+        <v>1.7038</v>
       </c>
       <c r="W46" t="n">
-        <v>-2.1177</v>
+        <v>-1.8413</v>
       </c>
     </row>
     <row r="47">
@@ -3812,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="n">
-        <v>0</v>
+        <v>0.0014</v>
       </c>
       <c r="O47" t="n">
         <v>0</v>
@@ -3886,19 +3886,19 @@
         <v>0</v>
       </c>
       <c r="O48" t="n">
-        <v>-0.0046</v>
+        <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>-0.0044</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="n">
-        <v>-0.0043</v>
+        <v>0</v>
       </c>
       <c r="R48" t="n">
-        <v>-0.0042</v>
+        <v>0</v>
       </c>
       <c r="S48" t="n">
-        <v>-0.0041</v>
+        <v>0</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -4022,37 +4022,37 @@
         <v>0</v>
       </c>
       <c r="M50" t="n">
-        <v>-0.0638</v>
+        <v>0</v>
       </c>
       <c r="N50" t="n">
-        <v>0.1652</v>
+        <v>-0.006</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.1987</v>
+        <v>-0.2055</v>
       </c>
       <c r="P50" t="n">
-        <v>-0.0019</v>
+        <v>0</v>
       </c>
       <c r="Q50" t="n">
-        <v>-0.0027</v>
+        <v>0</v>
       </c>
       <c r="R50" t="n">
-        <v>0.0101</v>
+        <v>-0.0001</v>
       </c>
       <c r="S50" t="n">
-        <v>0.0053</v>
+        <v>0</v>
       </c>
       <c r="T50" t="n">
-        <v>-0.0013</v>
+        <v>0</v>
       </c>
       <c r="U50" t="n">
-        <v>0.0007</v>
+        <v>0</v>
       </c>
       <c r="V50" t="n">
-        <v>41.8988</v>
+        <v>41.8903</v>
       </c>
       <c r="W50" t="n">
-        <v>-43.2179</v>
+        <v>-41.593</v>
       </c>
     </row>
     <row r="51">
@@ -4093,37 +4093,37 @@
         <v>0</v>
       </c>
       <c r="M51" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="N51" t="n">
-        <v>-0.0009</v>
+        <v>0.0002</v>
       </c>
       <c r="O51" t="n">
-        <v>-0.0016</v>
+        <v>0.0002</v>
       </c>
       <c r="P51" t="n">
-        <v>-0.0013</v>
+        <v>0.0002</v>
       </c>
       <c r="Q51" t="n">
-        <v>-0.0006</v>
+        <v>0.0002</v>
       </c>
       <c r="R51" t="n">
-        <v>0.0001</v>
+        <v>0.0002</v>
       </c>
       <c r="S51" t="n">
-        <v>-0.0008</v>
+        <v>0.0002</v>
       </c>
       <c r="T51" t="n">
-        <v>-0.0008</v>
+        <v>0.0002</v>
       </c>
       <c r="U51" t="n">
-        <v>-0.0006</v>
+        <v>0.0002</v>
       </c>
       <c r="V51" t="n">
-        <v>-0.0007</v>
+        <v>-0.0002</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0019</v>
+        <v>-0.0002</v>
       </c>
     </row>
     <row r="52">
@@ -4164,37 +4164,37 @@
         <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.0405</v>
+        <v>0</v>
       </c>
       <c r="N52" t="n">
-        <v>-0.039</v>
+        <v>-0.0419</v>
       </c>
       <c r="O52" t="n">
-        <v>-0.0047</v>
+        <v>-0.0089</v>
       </c>
       <c r="P52" t="n">
-        <v>0.0054</v>
+        <v>0.0036</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.05</v>
+        <v>0.0025</v>
       </c>
       <c r="R52" t="n">
-        <v>0.0412</v>
+        <v>0.0415</v>
       </c>
       <c r="S52" t="n">
-        <v>0.0081</v>
+        <v>0.009</v>
       </c>
       <c r="T52" t="n">
-        <v>-0.0046</v>
+        <v>-0.0039</v>
       </c>
       <c r="U52" t="n">
-        <v>-0.0032</v>
+        <v>-0.0029</v>
       </c>
       <c r="V52" t="n">
+        <v>0.0028</v>
+      </c>
+      <c r="W52" t="n">
         <v>0.003</v>
-      </c>
-      <c r="W52" t="n">
-        <v>-0.0361</v>
       </c>
     </row>
     <row r="53">
@@ -4235,37 +4235,37 @@
         <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>0.0594</v>
+        <v>0</v>
       </c>
       <c r="N53" t="n">
-        <v>0.0562</v>
+        <v>0.069</v>
       </c>
       <c r="O53" t="n">
-        <v>0.0347</v>
+        <v>0.0682</v>
       </c>
       <c r="P53" t="n">
-        <v>0.0336</v>
+        <v>0.0338</v>
       </c>
       <c r="Q53" t="n">
-        <v>0.0318</v>
+        <v>0.0334</v>
       </c>
       <c r="R53" t="n">
-        <v>0.0297</v>
+        <v>0.0331</v>
       </c>
       <c r="S53" t="n">
-        <v>0.0262</v>
+        <v>0.0328</v>
       </c>
       <c r="T53" t="n">
-        <v>0.0271</v>
+        <v>0.0324</v>
       </c>
       <c r="U53" t="n">
-        <v>-0.0009</v>
+        <v>0.0321</v>
       </c>
       <c r="V53" t="n">
-        <v>-0.0207</v>
+        <v>-0.0197</v>
       </c>
       <c r="W53" t="n">
-        <v>0.0875</v>
+        <v>-0.0802</v>
       </c>
     </row>
     <row r="54">
@@ -4306,10 +4306,10 @@
         <v>0</v>
       </c>
       <c r="M54" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="N54" t="n">
-        <v>0.0003</v>
+        <v>0.0015</v>
       </c>
       <c r="O54" t="n">
         <v>0.0015</v>
@@ -4380,7 +4380,7 @@
         <v>0</v>
       </c>
       <c r="N55" t="n">
-        <v>0</v>
+        <v>-18.3983</v>
       </c>
       <c r="O55" t="n">
         <v>0</v>
@@ -4451,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="O56" t="n">
         <v>-0.0001</v>
@@ -4466,16 +4466,16 @@
         <v>0</v>
       </c>
       <c r="S56" t="n">
+        <v>0</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0</v>
+      </c>
+      <c r="U56" t="n">
+        <v>0</v>
+      </c>
+      <c r="V56" t="n">
         <v>-0.0001</v>
-      </c>
-      <c r="T56" t="n">
-        <v>0</v>
-      </c>
-      <c r="U56" t="n">
-        <v>0</v>
-      </c>
-      <c r="V56" t="n">
-        <v>0</v>
       </c>
       <c r="W56" t="n">
         <v>0</v>
@@ -4522,34 +4522,34 @@
         <v>0</v>
       </c>
       <c r="N57" t="n">
+        <v>-0.0015</v>
+      </c>
+      <c r="O57" t="n">
         <v>0.0001</v>
       </c>
-      <c r="O57" t="n">
-        <v>0.0002</v>
-      </c>
       <c r="P57" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q57" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="R57" t="n">
         <v>0.0003</v>
       </c>
       <c r="S57" t="n">
-        <v>0.0003</v>
+        <v>0.0002</v>
       </c>
       <c r="T57" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="U57" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="V57" t="n">
-        <v>0.0717</v>
+        <v>0.0719</v>
       </c>
       <c r="W57" t="n">
-        <v>-0.014</v>
+        <v>-0.0109</v>
       </c>
     </row>
     <row r="58">

</xml_diff>

<commit_message>
data: replace resultts 04-2024 folder with "as-published" results
</commit_message>
<xml_diff>
--- a/results/04-2024/comparison-deflators-04-2024.xlsx
+++ b/results/04-2024/comparison-deflators-04-2024.xlsx
@@ -644,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0.0051</v>
+        <v>0.0052</v>
       </c>
     </row>
     <row r="3">
@@ -691,31 +691,31 @@
         <v>310.9897</v>
       </c>
       <c r="O3" t="n">
-        <v>311.58</v>
+        <v>315.355</v>
       </c>
       <c r="P3" t="n">
-        <v>313.653</v>
+        <v>317.119</v>
       </c>
       <c r="Q3" t="n">
-        <v>315.562</v>
+        <v>318.802</v>
       </c>
       <c r="R3" t="n">
-        <v>317.539</v>
+        <v>320.534</v>
       </c>
       <c r="S3" t="n">
-        <v>319.487</v>
+        <v>322.229</v>
       </c>
       <c r="T3" t="n">
-        <v>321.422</v>
+        <v>323.907</v>
       </c>
       <c r="U3" t="n">
-        <v>323.328</v>
+        <v>325.59</v>
       </c>
       <c r="V3" t="n">
-        <v>325.189</v>
+        <v>327.231</v>
       </c>
       <c r="W3" t="n">
-        <v>327.004</v>
+        <v>328.868</v>
       </c>
     </row>
     <row r="4">
@@ -765,25 +765,25 @@
         <v>-0.0177</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0671</v>
+        <v>-0.0669</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.0292</v>
+        <v>-0.029</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0283</v>
+        <v>-0.028</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.0267</v>
+        <v>-0.0264</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.026</v>
+        <v>-0.0257</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.0039</v>
+        <v>-0.0038</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.0027</v>
+        <v>-0.0026</v>
       </c>
       <c r="W4" t="n">
         <v>-0.0022</v>
@@ -833,31 +833,31 @@
         <v>-0.2668</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.5631</v>
+        <v>-0.3599</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.2754</v>
+        <v>-0.0673</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.2921</v>
+        <v>-0.0838</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.6339</v>
+        <v>-0.4221</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.5056</v>
+        <v>-0.2982</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.332</v>
+        <v>-0.1313</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.3637</v>
+        <v>-0.167</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.296</v>
+        <v>-0.106</v>
       </c>
       <c r="W5" t="n">
-        <v>-32.0709</v>
+        <v>-31.4048</v>
       </c>
     </row>
     <row r="6">
@@ -904,31 +904,31 @@
         <v>0.1561</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1297</v>
+        <v>-0.1203</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.247</v>
+        <v>-0.2381</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.2305</v>
+        <v>-0.2235</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2896</v>
+        <v>-0.2839</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2222</v>
+        <v>-0.2195</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.1704</v>
+        <v>-0.1707</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.0312</v>
+        <v>-0.0354</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1097</v>
+        <v>-0.1141</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.4258</v>
+        <v>-0.4273</v>
       </c>
     </row>
     <row r="7">
@@ -975,31 +975,31 @@
         <v>-0.2224</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.214</v>
+        <v>-0.1833</v>
       </c>
       <c r="P7" t="n">
-        <v>-0.0229</v>
+        <v>0.0393</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0949</v>
+        <v>-0.0011</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.0694</v>
+        <v>0.0551</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.0808</v>
+        <v>0.0448</v>
       </c>
       <c r="T7" t="n">
-        <v>-0.0931</v>
+        <v>0.0321</v>
       </c>
       <c r="U7" t="n">
-        <v>-0.0754</v>
+        <v>0.0484</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.0293</v>
+        <v>0.092</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.2202</v>
+        <v>-5.0242</v>
       </c>
     </row>
     <row r="8">
@@ -1046,31 +1046,31 @@
         <v>0.2014</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1562</v>
+        <v>0.11</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3677</v>
+        <v>0.273</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.328</v>
+        <v>0.2087</v>
       </c>
       <c r="R8" t="n">
-        <v>0.006</v>
+        <v>-0.1338</v>
       </c>
       <c r="S8" t="n">
-        <v>0.0105</v>
+        <v>-0.1517</v>
       </c>
       <c r="T8" t="n">
-        <v>0.06</v>
+        <v>-0.1241</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0872</v>
+        <v>-0.1174</v>
       </c>
       <c r="V8" t="n">
-        <v>0.1572</v>
+        <v>-0.0675</v>
       </c>
       <c r="W8" t="n">
-        <v>7.7984</v>
+        <v>7.4628</v>
       </c>
     </row>
     <row r="9">
@@ -1117,31 +1117,31 @@
         <v>-0.0373</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0358</v>
+        <v>-0.0357</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0345</v>
+        <v>-0.0344</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.0226</v>
+        <v>-0.0224</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0154</v>
+        <v>-0.0152</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.014</v>
+        <v>-0.0138</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.0141</v>
+        <v>-0.0139</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.0132</v>
+        <v>-0.0129</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.0145</v>
+        <v>-0.0143</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.01</v>
+        <v>-0.0097</v>
       </c>
     </row>
     <row r="10">
@@ -1188,31 +1188,31 @@
         <v>-0.062</v>
       </c>
       <c r="O10" t="n">
-        <v>-0.0489</v>
+        <v>-0.0488</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.0436</v>
+        <v>-0.0433</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0261</v>
+        <v>-0.0258</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0106</v>
+        <v>-0.0103</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0101</v>
+        <v>-0.0098</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.0086</v>
+        <v>-0.0083</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.0078</v>
+        <v>-0.0075</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.0072</v>
+        <v>-0.0069</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.0065</v>
+        <v>-0.0063</v>
       </c>
     </row>
     <row r="11">
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0058</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="12">
@@ -1330,31 +1330,31 @@
         <v>-0.0659</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0157</v>
+        <v>0.0242</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0141</v>
+        <v>0.0661</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0501</v>
+        <v>0.0699</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.2203</v>
+        <v>-0.0599</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.2158</v>
+        <v>-0.0547</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.2139</v>
+        <v>-0.054</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.2669</v>
+        <v>-0.1083</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.2234</v>
+        <v>-0.0687</v>
       </c>
       <c r="W12" t="n">
-        <v>-6.5828</v>
+        <v>-6.3375</v>
       </c>
     </row>
     <row r="13">
@@ -1404,28 +1404,28 @@
         <v>-0.0932</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.0552</v>
+        <v>-0.0549</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.0302</v>
+        <v>-0.0298</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.0299</v>
+        <v>-0.0295</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.0237</v>
+        <v>-0.0232</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.0003</v>
+        <v>-0.0001</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.0074</v>
+        <v>-0.0071</v>
       </c>
     </row>
     <row r="14">
@@ -1472,31 +1472,31 @@
         <v>-0.1042</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.2924</v>
+        <v>-0.292</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2645</v>
+        <v>-0.2628</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1078</v>
+        <v>-0.106</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0601</v>
+        <v>-0.0581</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0955</v>
+        <v>-0.0926</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0716</v>
+        <v>-0.0687</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.0334</v>
+        <v>-0.0308</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0142</v>
+        <v>-0.0116</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.0762</v>
+        <v>-0.0725</v>
       </c>
     </row>
     <row r="15">
@@ -1614,31 +1614,31 @@
         <v>-0.2545</v>
       </c>
       <c r="O16" t="n">
-        <v>-1.1215</v>
+        <v>-0.6738</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.834</v>
+        <v>-0.363</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.6318</v>
+        <v>-0.119</v>
       </c>
       <c r="R16" t="n">
-        <v>-1.2479</v>
+        <v>-0.6862</v>
       </c>
       <c r="S16" t="n">
-        <v>-1.3453</v>
+        <v>-0.8195</v>
       </c>
       <c r="T16" t="n">
-        <v>-1.0426</v>
+        <v>-0.5642</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.8006</v>
+        <v>-0.3704</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.4689</v>
+        <v>-0.0909</v>
       </c>
       <c r="W16" t="n">
-        <v>-72.0796</v>
+        <v>-70.6471</v>
       </c>
     </row>
     <row r="17">
@@ -1685,31 +1685,31 @@
         <v>28284.5</v>
       </c>
       <c r="O17" t="n">
-        <v>28521.5094</v>
+        <v>28622.474</v>
       </c>
       <c r="P17" t="n">
-        <v>28783.7326</v>
+        <v>28967.3369</v>
       </c>
       <c r="Q17" t="n">
-        <v>29054.2258</v>
+        <v>29324.412</v>
       </c>
       <c r="R17" t="n">
-        <v>29343.8816</v>
+        <v>29688.2716</v>
       </c>
       <c r="S17" t="n">
-        <v>29655.9272</v>
+        <v>30043.4679</v>
       </c>
       <c r="T17" t="n">
-        <v>29972.2086</v>
+        <v>30393.654</v>
       </c>
       <c r="U17" t="n">
-        <v>30298.979</v>
+        <v>30731.3149</v>
       </c>
       <c r="V17" t="n">
-        <v>30607.7972</v>
+        <v>31069.1846</v>
       </c>
       <c r="W17" t="n">
-        <v>30918.9351</v>
+        <v>31411.9599</v>
       </c>
     </row>
     <row r="18">
@@ -1756,31 +1756,31 @@
         <v>-0.1094</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.2544</v>
+        <v>-0.2106</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0547</v>
+        <v>-0.0107</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.0286</v>
+        <v>0.0152</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.3518</v>
+        <v>-0.3049</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.2338</v>
+        <v>-0.1896</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.0771</v>
+        <v>-0.0365</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.128</v>
+        <v>-0.0876</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.0304</v>
+        <v>0.0072</v>
       </c>
       <c r="W18" t="n">
-        <v>-6.4464</v>
+        <v>-6.3151</v>
       </c>
     </row>
     <row r="19">
@@ -1827,31 +1827,31 @@
         <v>0.0055</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0103</v>
+        <v>0.0041</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0105</v>
+        <v>0.0042</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.0106</v>
+        <v>0.0043</v>
       </c>
       <c r="R19" t="n">
-        <v>0.0107</v>
+        <v>0.0043</v>
       </c>
       <c r="S19" t="n">
-        <v>0.0106</v>
+        <v>0.0044</v>
       </c>
       <c r="T19" t="n">
-        <v>0.0106</v>
+        <v>0.0044</v>
       </c>
       <c r="U19" t="n">
-        <v>0.0105</v>
+        <v>0.0045</v>
       </c>
       <c r="V19" t="n">
-        <v>0.0104</v>
+        <v>0.0045</v>
       </c>
       <c r="W19" t="n">
-        <v>0.0103</v>
+        <v>0.0045</v>
       </c>
     </row>
     <row r="20">
@@ -1901,16 +1901,16 @@
         <v>-0.105</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.1023</v>
+        <v>-0.1019</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.1004</v>
+        <v>-0.0998</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.0976</v>
+        <v>-0.0967</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.0948</v>
+        <v>-0.0937</v>
       </c>
       <c r="T20" t="n">
         <v>-0.001</v>
@@ -1919,7 +1919,7 @@
         <v>-0.001</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.001</v>
+        <v>-0.0009</v>
       </c>
       <c r="W20" t="n">
         <v>0</v>
@@ -2040,31 +2040,31 @@
         <v>0.0936</v>
       </c>
       <c r="O22" t="n">
-        <v>-0.069</v>
+        <v>0.1557</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.277</v>
+        <v>-0.0437</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.2961</v>
+        <v>-0.0625</v>
       </c>
       <c r="R22" t="n">
-        <v>0.0014</v>
+        <v>0.2326</v>
       </c>
       <c r="S22" t="n">
-        <v>-0.1108</v>
+        <v>0.1211</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.2602</v>
+        <v>-0.0292</v>
       </c>
       <c r="U22" t="n">
-        <v>-0.2099</v>
+        <v>0.0161</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.0235</v>
+        <v>0.1944</v>
       </c>
       <c r="W22" t="n">
-        <v>-37.8912</v>
+        <v>-37.1192</v>
       </c>
     </row>
     <row r="23">
@@ -2111,31 +2111,31 @@
         <v>-0.02</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.0156</v>
+        <v>-0.016</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.0076</v>
+        <v>-0.0085</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.0097</v>
+        <v>0.0083</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0245</v>
+        <v>0.0225</v>
       </c>
       <c r="S23" t="n">
-        <v>0.0045</v>
+        <v>0.0022</v>
       </c>
       <c r="T23" t="n">
-        <v>0.005</v>
+        <v>0.0023</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0106</v>
+        <v>0.0074</v>
       </c>
       <c r="V23" t="n">
-        <v>0.0155</v>
+        <v>0.0118</v>
       </c>
       <c r="W23" t="n">
-        <v>0.0778</v>
+        <v>0.0729</v>
       </c>
     </row>
     <row r="24">
@@ -2182,31 +2182,31 @@
         <v>0.1087</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0221</v>
+        <v>0.0277</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.039</v>
+        <v>-0.0275</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.0807</v>
+        <v>0.0972</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0288</v>
+        <v>-0.006</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.0428</v>
+        <v>-0.0198</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.038</v>
+        <v>-0.0153</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.03</v>
+        <v>-0.0077</v>
       </c>
       <c r="V24" t="n">
-        <v>-0.017</v>
+        <v>0.0047</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.9285</v>
+        <v>-0.8938</v>
       </c>
     </row>
     <row r="25">
@@ -2253,31 +2253,31 @@
         <v>0.2383</v>
       </c>
       <c r="O25" t="n">
-        <v>0.2549</v>
+        <v>0.2312</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1959</v>
+        <v>0.1473</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.172</v>
+        <v>0.1108</v>
       </c>
       <c r="R25" t="n">
-        <v>0.142</v>
+        <v>0.0689</v>
       </c>
       <c r="S25" t="n">
-        <v>0.0786</v>
+        <v>-0.0054</v>
       </c>
       <c r="T25" t="n">
-        <v>0.1177</v>
+        <v>0.0223</v>
       </c>
       <c r="U25" t="n">
-        <v>0.1369</v>
+        <v>0.0307</v>
       </c>
       <c r="V25" t="n">
-        <v>0.0935</v>
+        <v>-0.022</v>
       </c>
       <c r="W25" t="n">
-        <v>4.0038</v>
+        <v>3.8316</v>
       </c>
     </row>
     <row r="26">
@@ -2348,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="W26" t="n">
-        <v>0.0067</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="27">
@@ -2481,7 +2481,7 @@
         <v>-0.0013</v>
       </c>
       <c r="T28" t="n">
-        <v>-0.0004</v>
+        <v>-0.0003</v>
       </c>
       <c r="U28" t="n">
         <v>-0.0003</v>
@@ -2537,31 +2537,31 @@
         <v>-0.0027</v>
       </c>
       <c r="O29" t="n">
-        <v>0.004</v>
+        <v>0.0044</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0053</v>
+        <v>0.0061</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0046</v>
+        <v>0.0057</v>
       </c>
       <c r="R29" t="n">
-        <v>0.0048</v>
+        <v>0.0062</v>
       </c>
       <c r="S29" t="n">
-        <v>0.0047</v>
+        <v>0.0063</v>
       </c>
       <c r="T29" t="n">
-        <v>0.0032</v>
+        <v>0.0049</v>
       </c>
       <c r="U29" t="n">
-        <v>0.0005</v>
+        <v>0.0024</v>
       </c>
       <c r="V29" t="n">
-        <v>-0.0006</v>
+        <v>0.0013</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.0742</v>
+        <v>-0.0712</v>
       </c>
     </row>
     <row r="30">
@@ -2679,31 +2679,31 @@
         <v>-2.4563</v>
       </c>
       <c r="O31" t="n">
-        <v>-3.775</v>
+        <v>0</v>
       </c>
       <c r="P31" t="n">
-        <v>-3.466</v>
+        <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>-3.24</v>
+        <v>0</v>
       </c>
       <c r="R31" t="n">
-        <v>-2.995</v>
+        <v>0</v>
       </c>
       <c r="S31" t="n">
-        <v>-2.742</v>
+        <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>-2.485</v>
+        <v>0</v>
       </c>
       <c r="U31" t="n">
-        <v>-2.262</v>
+        <v>0</v>
       </c>
       <c r="V31" t="n">
-        <v>-2.042</v>
+        <v>0</v>
       </c>
       <c r="W31" t="n">
-        <v>-1.864</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2753,22 +2753,22 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="S32" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="V32" t="n">
         <v>0</v>
@@ -2821,31 +2821,31 @@
         <v>-0.0109</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.1008</v>
+        <v>0.1024</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.2084</v>
+        <v>-0.0004</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.2089</v>
+        <v>-0.0006</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.2124</v>
+        <v>-0.0006</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.208</v>
+        <v>-0.0006</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.2013</v>
+        <v>-0.0006</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.1973</v>
+        <v>-0.0005</v>
       </c>
       <c r="V33" t="n">
-        <v>1.6471</v>
+        <v>1.8371</v>
       </c>
       <c r="W33" t="n">
-        <v>-2.6195</v>
+        <v>-1.9534</v>
       </c>
     </row>
     <row r="34">
@@ -2892,31 +2892,31 @@
         <v>-0.0031</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0089</v>
+        <v>0.0005</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.0083</v>
+        <v>0.0005</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.0064</v>
+        <v>0.0005</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.0052</v>
+        <v>0.0005</v>
       </c>
       <c r="S34" t="n">
-        <v>-0.0022</v>
+        <v>0.0005</v>
       </c>
       <c r="T34" t="n">
-        <v>0.0007</v>
+        <v>0.0005</v>
       </c>
       <c r="U34" t="n">
-        <v>0.0047</v>
+        <v>0.0004</v>
       </c>
       <c r="V34" t="n">
-        <v>0.6324</v>
+        <v>0.628</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.6233</v>
+        <v>-0.6247</v>
       </c>
     </row>
     <row r="35">
@@ -2963,31 +2963,31 @@
         <v>0.0102</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0053</v>
+        <v>0.036</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.003</v>
+        <v>0.0592</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.038</v>
+        <v>0.0558</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.0818</v>
+        <v>0.0428</v>
       </c>
       <c r="S35" t="n">
-        <v>-0.1107</v>
+        <v>0.0149</v>
       </c>
       <c r="T35" t="n">
-        <v>-0.1357</v>
+        <v>-0.0104</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.1314</v>
+        <v>-0.0075</v>
       </c>
       <c r="V35" t="n">
-        <v>-0.0995</v>
+        <v>0.0218</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.2308</v>
+        <v>-0.0348</v>
       </c>
     </row>
     <row r="36">
@@ -3034,31 +3034,31 @@
         <v>-0.0438</v>
       </c>
       <c r="O36" t="n">
-        <v>-0.0511</v>
+        <v>-0.0973</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0204</v>
+        <v>-0.0743</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0726</v>
+        <v>-0.0467</v>
       </c>
       <c r="R36" t="n">
-        <v>0.0927</v>
+        <v>-0.0472</v>
       </c>
       <c r="S36" t="n">
-        <v>0.1158</v>
+        <v>-0.0464</v>
       </c>
       <c r="T36" t="n">
-        <v>0.139</v>
+        <v>-0.045</v>
       </c>
       <c r="U36" t="n">
-        <v>0.1602</v>
+        <v>-0.0443</v>
       </c>
       <c r="V36" t="n">
-        <v>0.1606</v>
+        <v>-0.064</v>
       </c>
       <c r="W36" t="n">
-        <v>0.4071</v>
+        <v>0.0715</v>
       </c>
     </row>
     <row r="37">
@@ -3108,28 +3108,28 @@
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="S37" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="T37" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="U37" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="W37" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3176,31 +3176,31 @@
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="P38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="R38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="S38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="T38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="U38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="V38" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="W38" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3271,7 +3271,7 @@
         <v>-0.0053</v>
       </c>
       <c r="W39" t="n">
-        <v>0.0004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -3318,31 +3318,31 @@
         <v>0.1071</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0646</v>
+        <v>0.1045</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0218</v>
+        <v>0.1021</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0203</v>
+        <v>0.0997</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.164</v>
+        <v>-0.0036</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.1645</v>
+        <v>-0.0034</v>
       </c>
       <c r="T40" t="n">
-        <v>-0.1632</v>
+        <v>-0.0034</v>
       </c>
       <c r="U40" t="n">
-        <v>-0.162</v>
+        <v>-0.0033</v>
       </c>
       <c r="V40" t="n">
-        <v>6.0813</v>
+        <v>6.236</v>
       </c>
       <c r="W40" t="n">
-        <v>-0.3857</v>
+        <v>-0.1405</v>
       </c>
     </row>
     <row r="41">
@@ -3392,28 +3392,28 @@
         <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="R41" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="S41" t="n">
-        <v>-0.0004</v>
+        <v>0</v>
       </c>
       <c r="T41" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="U41" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="V41" t="n">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c r="W41" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3460,31 +3460,31 @@
         <v>-0.0007</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.0019</v>
+        <v>-0.0015</v>
       </c>
       <c r="P42" t="n">
-        <v>-0.003</v>
+        <v>-0.0013</v>
       </c>
       <c r="Q42" t="n">
-        <v>-0.003</v>
+        <v>-0.0012</v>
       </c>
       <c r="R42" t="n">
-        <v>-0.0031</v>
+        <v>-0.0011</v>
       </c>
       <c r="S42" t="n">
-        <v>-0.0038</v>
+        <v>-0.001</v>
       </c>
       <c r="T42" t="n">
-        <v>-0.0039</v>
+        <v>-0.001</v>
       </c>
       <c r="U42" t="n">
-        <v>-0.0036</v>
+        <v>-0.001</v>
       </c>
       <c r="V42" t="n">
-        <v>0.0636</v>
+        <v>0.0662</v>
       </c>
       <c r="W42" t="n">
-        <v>-0.0124</v>
+        <v>-0.0087</v>
       </c>
     </row>
     <row r="43">
@@ -3602,31 +3602,31 @@
         <v>0.0184</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.4495</v>
+        <v>-0.0019</v>
       </c>
       <c r="P44" t="n">
-        <v>-0.3483</v>
+        <v>0.1226</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.3698</v>
+        <v>0.143</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.4388</v>
+        <v>0.1229</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.5197</v>
+        <v>0.0061</v>
       </c>
       <c r="T44" t="n">
-        <v>-0.5097</v>
+        <v>-0.0312</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.457</v>
+        <v>-0.0269</v>
       </c>
       <c r="V44" t="n">
-        <v>50.2955</v>
+        <v>50.6734</v>
       </c>
       <c r="W44" t="n">
-        <v>-45.8008</v>
+        <v>-44.3683</v>
       </c>
     </row>
     <row r="45">
@@ -3673,31 +3673,31 @@
         <v>7.7756</v>
       </c>
       <c r="O45" t="n">
-        <v>-93.0961</v>
+        <v>7.8685</v>
       </c>
       <c r="P45" t="n">
-        <v>-175.6411</v>
+        <v>7.9633</v>
       </c>
       <c r="Q45" t="n">
-        <v>-262.1247</v>
+        <v>8.0615</v>
       </c>
       <c r="R45" t="n">
-        <v>-336.2285</v>
+        <v>8.1615</v>
       </c>
       <c r="S45" t="n">
-        <v>-379.2816</v>
+        <v>8.2591</v>
       </c>
       <c r="T45" t="n">
-        <v>-413.09</v>
+        <v>8.3554</v>
       </c>
       <c r="U45" t="n">
-        <v>-423.8877</v>
+        <v>8.4482</v>
       </c>
       <c r="V45" t="n">
-        <v>-452.8462</v>
+        <v>8.5411</v>
       </c>
       <c r="W45" t="n">
-        <v>-484.3895</v>
+        <v>8.6353</v>
       </c>
     </row>
     <row r="46">
@@ -3744,31 +3744,31 @@
         <v>0.0097</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0973</v>
+        <v>0.1411</v>
       </c>
       <c r="P46" t="n">
-        <v>-0.0441</v>
+        <v>-0.0001</v>
       </c>
       <c r="Q46" t="n">
-        <v>-0.044</v>
+        <v>-0.0001</v>
       </c>
       <c r="R46" t="n">
-        <v>-0.0471</v>
+        <v>-0.0001</v>
       </c>
       <c r="S46" t="n">
-        <v>-0.0443</v>
+        <v>-0.0001</v>
       </c>
       <c r="T46" t="n">
-        <v>-0.0408</v>
+        <v>-0.0002</v>
       </c>
       <c r="U46" t="n">
-        <v>-0.0406</v>
+        <v>-0.0002</v>
       </c>
       <c r="V46" t="n">
-        <v>1.6662</v>
+        <v>1.7038</v>
       </c>
       <c r="W46" t="n">
-        <v>-1.9726</v>
+        <v>-1.8413</v>
       </c>
     </row>
     <row r="47">
@@ -3815,31 +3815,31 @@
         <v>0.0014</v>
       </c>
       <c r="O47" t="n">
-        <v>0.0061</v>
+        <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>0.0063</v>
+        <v>0</v>
       </c>
       <c r="Q47" t="n">
-        <v>0.0063</v>
+        <v>0</v>
       </c>
       <c r="R47" t="n">
-        <v>0.0063</v>
+        <v>0</v>
       </c>
       <c r="S47" t="n">
-        <v>0.0063</v>
+        <v>0</v>
       </c>
       <c r="T47" t="n">
-        <v>0.0062</v>
+        <v>0</v>
       </c>
       <c r="U47" t="n">
-        <v>0.0061</v>
+        <v>0</v>
       </c>
       <c r="V47" t="n">
-        <v>0.0059</v>
+        <v>0</v>
       </c>
       <c r="W47" t="n">
-        <v>0.0058</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -3889,16 +3889,16 @@
         <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="n">
-        <v>-0.0006</v>
+        <v>0</v>
       </c>
       <c r="R48" t="n">
-        <v>-0.0009</v>
+        <v>0</v>
       </c>
       <c r="S48" t="n">
-        <v>-0.0011</v>
+        <v>0</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -4028,31 +4028,31 @@
         <v>-0.006</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.4302</v>
+        <v>-0.2055</v>
       </c>
       <c r="P50" t="n">
-        <v>-0.2333</v>
+        <v>0</v>
       </c>
       <c r="Q50" t="n">
-        <v>-0.2336</v>
+        <v>0</v>
       </c>
       <c r="R50" t="n">
-        <v>-0.2313</v>
+        <v>-0.0001</v>
       </c>
       <c r="S50" t="n">
-        <v>-0.2319</v>
+        <v>0</v>
       </c>
       <c r="T50" t="n">
-        <v>-0.231</v>
+        <v>0</v>
       </c>
       <c r="U50" t="n">
-        <v>-0.2259</v>
+        <v>0</v>
       </c>
       <c r="V50" t="n">
-        <v>41.6724</v>
+        <v>41.8903</v>
       </c>
       <c r="W50" t="n">
-        <v>-42.365</v>
+        <v>-41.593</v>
       </c>
     </row>
     <row r="51">
@@ -4099,31 +4099,31 @@
         <v>0.0002</v>
       </c>
       <c r="O51" t="n">
-        <v>0.0006</v>
+        <v>0.0002</v>
       </c>
       <c r="P51" t="n">
-        <v>0.0011</v>
+        <v>0.0002</v>
       </c>
       <c r="Q51" t="n">
-        <v>0.0016</v>
+        <v>0.0002</v>
       </c>
       <c r="R51" t="n">
-        <v>0.0022</v>
+        <v>0.0002</v>
       </c>
       <c r="S51" t="n">
-        <v>0.0025</v>
+        <v>0.0002</v>
       </c>
       <c r="T51" t="n">
-        <v>0.0029</v>
+        <v>0.0002</v>
       </c>
       <c r="U51" t="n">
-        <v>0.0034</v>
+        <v>0.0002</v>
       </c>
       <c r="V51" t="n">
-        <v>0.0034</v>
+        <v>-0.0002</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0047</v>
+        <v>-0.0002</v>
       </c>
     </row>
     <row r="52">
@@ -4170,31 +4170,31 @@
         <v>-0.0419</v>
       </c>
       <c r="O52" t="n">
-        <v>-0.0145</v>
+        <v>-0.0089</v>
       </c>
       <c r="P52" t="n">
-        <v>-0.0079</v>
+        <v>0.0036</v>
       </c>
       <c r="Q52" t="n">
-        <v>-0.014</v>
+        <v>0.0025</v>
       </c>
       <c r="R52" t="n">
-        <v>0.0187</v>
+        <v>0.0415</v>
       </c>
       <c r="S52" t="n">
-        <v>-0.0141</v>
+        <v>0.009</v>
       </c>
       <c r="T52" t="n">
-        <v>-0.0266</v>
+        <v>-0.0039</v>
       </c>
       <c r="U52" t="n">
-        <v>-0.0252</v>
+        <v>-0.0029</v>
       </c>
       <c r="V52" t="n">
-        <v>-0.0189</v>
+        <v>0.0028</v>
       </c>
       <c r="W52" t="n">
-        <v>-0.0317</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="53">
@@ -4241,31 +4241,31 @@
         <v>0.069</v>
       </c>
       <c r="O53" t="n">
-        <v>0.092</v>
+        <v>0.0682</v>
       </c>
       <c r="P53" t="n">
-        <v>0.0823</v>
+        <v>0.0338</v>
       </c>
       <c r="Q53" t="n">
-        <v>0.0946</v>
+        <v>0.0334</v>
       </c>
       <c r="R53" t="n">
-        <v>0.1062</v>
+        <v>0.0331</v>
       </c>
       <c r="S53" t="n">
-        <v>0.1168</v>
+        <v>0.0328</v>
       </c>
       <c r="T53" t="n">
-        <v>0.1279</v>
+        <v>0.0324</v>
       </c>
       <c r="U53" t="n">
-        <v>0.1383</v>
+        <v>0.0321</v>
       </c>
       <c r="V53" t="n">
-        <v>0.0958</v>
+        <v>-0.0197</v>
       </c>
       <c r="W53" t="n">
-        <v>0.092</v>
+        <v>-0.0802</v>
       </c>
     </row>
     <row r="54">
@@ -4336,7 +4336,7 @@
         <v>-0.0068</v>
       </c>
       <c r="W54" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="R56" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
@@ -4525,31 +4525,31 @@
         <v>-0.0015</v>
       </c>
       <c r="O57" t="n">
-        <v>-0.0003</v>
+        <v>0.0001</v>
       </c>
       <c r="P57" t="n">
-        <v>-0.0008</v>
+        <v>0</v>
       </c>
       <c r="Q57" t="n">
-        <v>-0.0011</v>
+        <v>0</v>
       </c>
       <c r="R57" t="n">
-        <v>-0.0011</v>
+        <v>0.0003</v>
       </c>
       <c r="S57" t="n">
-        <v>-0.0014</v>
+        <v>0.0002</v>
       </c>
       <c r="T57" t="n">
-        <v>-0.0018</v>
+        <v>0</v>
       </c>
       <c r="U57" t="n">
-        <v>-0.0018</v>
+        <v>0</v>
       </c>
       <c r="V57" t="n">
-        <v>0.0699</v>
+        <v>0.0719</v>
       </c>
       <c r="W57" t="n">
-        <v>-0.0139</v>
+        <v>-0.0109</v>
       </c>
     </row>
     <row r="58">

</xml_diff>